<commit_message>
modificacion en metodo upload database
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -70,7 +70,7 @@
     <t>ajuste_frentes_minimos</t>
   </si>
   <si>
-    <t>lllll</t>
+    <t>asd</t>
   </si>
   <si>
     <t>BOTELLA .5L</t>
@@ -716,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="9">
         <v>4</v>
@@ -772,7 +772,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="9">
         <v>1.5</v>
@@ -828,7 +828,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="9">
         <v>1</v>
@@ -884,7 +884,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="9">
         <v>1.5</v>
@@ -940,7 +940,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="9">
         <v>2</v>
@@ -1052,7 +1052,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="9">
         <v>2</v>
@@ -1108,7 +1108,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="9">
         <v>1.5</v>
@@ -1164,7 +1164,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="9">
         <v>2</v>
@@ -1220,7 +1220,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="9">
         <v>1.5</v>
@@ -1276,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -1310,7 +1310,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -1344,7 +1344,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -1400,7 +1400,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="9">
         <v>1</v>
@@ -1456,7 +1456,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -1512,7 +1512,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -1568,7 +1568,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -1624,7 +1624,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="9">
         <v>1</v>
@@ -1680,7 +1680,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -1736,7 +1736,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="9">
         <v>1.5</v>
@@ -1792,7 +1792,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>
@@ -1848,7 +1848,7 @@
         <v>24</v>
       </c>
       <c r="D23" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
@@ -1904,7 +1904,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="9">
         <v>1</v>

</xml_diff>